<commit_message>
Cambiato M = 10
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\sorting_hardware_accelerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C0DCAF-C0CA-4188-A007-3E3476003769}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21237558-9CFB-4656-8F9B-06178367A4E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E8EC0F0A-2AEE-4483-92F4-B556AB8AE888}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>N</t>
   </si>
@@ -48,15 +48,9 @@
     <t>Dynamic PC</t>
   </si>
   <si>
-    <t>188,71 MHz</t>
-  </si>
-  <si>
     <t>93 mW</t>
   </si>
   <si>
-    <t>5 mW</t>
-  </si>
-  <si>
     <t>95 mW</t>
   </si>
   <si>
@@ -72,18 +66,9 @@
     <t>Max Delay</t>
   </si>
   <si>
-    <t>4,755 ns</t>
-  </si>
-  <si>
     <t>ND</t>
   </si>
   <si>
-    <t>182,28 MHz</t>
-  </si>
-  <si>
-    <t>171,96 MHz</t>
-  </si>
-  <si>
     <t>6 mW</t>
   </si>
   <si>
@@ -96,18 +81,6 @@
     <t>212,26 MHz</t>
   </si>
   <si>
-    <t>4,804 ns</t>
-  </si>
-  <si>
-    <t>7 mW</t>
-  </si>
-  <si>
-    <t>5,119 ns</t>
-  </si>
-  <si>
-    <t>12 mW</t>
-  </si>
-  <si>
     <t>186,95 MHz</t>
   </si>
   <si>
@@ -132,9 +105,6 @@
     <t>33 mW</t>
   </si>
   <si>
-    <t>136,407 MHz</t>
-  </si>
-  <si>
     <t>7,173 ns</t>
   </si>
   <si>
@@ -151,6 +121,24 @@
   </si>
   <si>
     <t>147 mW</t>
+  </si>
+  <si>
+    <t>202,75 Mhz</t>
+  </si>
+  <si>
+    <t>136,4 MHz</t>
+  </si>
+  <si>
+    <t>4,634 ns</t>
+  </si>
+  <si>
+    <t>176,08 MHz</t>
+  </si>
+  <si>
+    <t>17 mW</t>
+  </si>
+  <si>
+    <t>5,338 ns</t>
   </si>
 </sst>
 </file>
@@ -527,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA926D9-B2BE-4BCD-90ED-74AA28F6FB5D}">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,10 +548,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>2</v>
@@ -572,10 +560,10 @@
         <v>3</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -583,25 +571,25 @@
         <v>8</v>
       </c>
       <c r="C3" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M3" s="2">
+        <v>11</v>
+      </c>
+      <c r="M3" s="3">
         <v>0.2</v>
       </c>
       <c r="N3" s="2">
-        <v>5.1999999999999998E-3</v>
+        <v>9.1000000000000004E-3</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -609,25 +597,25 @@
         <v>16</v>
       </c>
       <c r="C5" s="1">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="K5" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="M5" s="3">
         <v>0.36</v>
       </c>
       <c r="N5" s="2">
-        <v>8.0999999999999996E-3</v>
+        <v>1.52E-2</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -635,25 +623,25 @@
         <v>32</v>
       </c>
       <c r="C7" s="1">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="K7" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="M7" s="3">
         <v>0.68</v>
       </c>
       <c r="N7" s="2">
-        <v>1.38E-2</v>
+        <v>2.63E-2</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -662,30 +650,30 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="4">
         <v>1.32</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -693,25 +681,25 @@
         <v>8</v>
       </c>
       <c r="C11" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="M11" s="3">
         <v>0.2</v>
       </c>
       <c r="N11" s="2">
-        <v>9.1000000000000004E-3</v>
+        <v>1.5900000000000001E-2</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -719,25 +707,25 @@
         <v>8</v>
       </c>
       <c r="C13" s="1">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="M13" s="3">
         <v>0.2</v>
       </c>
       <c r="N13" s="2">
-        <v>1.5900000000000001E-2</v>
+        <v>3.6600000000000001E-2</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -745,25 +733,25 @@
         <v>8</v>
       </c>
       <c r="C15" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="M15" s="3">
         <v>0.2</v>
       </c>
       <c r="N15" s="2">
-        <v>3.6600000000000001E-2</v>
+        <v>7.6100000000000001E-2</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -771,108 +759,82 @@
         <v>8</v>
       </c>
       <c r="C17" s="1">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M17" s="3">
         <v>0.2</v>
       </c>
       <c r="N17" s="2">
-        <v>7.6100000000000001E-2</v>
+        <v>0.35239999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1">
+        <v>100</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0.68</v>
+      </c>
+      <c r="N19" s="2">
+        <v>0.24729999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>32</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5">
         <v>500</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M19" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="N19" s="2">
-        <v>0.35239999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>32</v>
-      </c>
-      <c r="C21" s="1">
-        <v>100</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M21" s="3">
+      <c r="D21" s="5"/>
+      <c r="E21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="4">
         <v>0.68</v>
       </c>
-      <c r="N21" s="2">
-        <v>0.24729999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
-        <v>32</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5">
-        <v>500</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L23" s="5"/>
-      <c r="M23" s="4">
-        <v>0.68</v>
-      </c>
-      <c r="N23" s="6">
+      <c r="N21" s="6">
         <v>1.2123999999999999</v>
       </c>
     </row>

</xml_diff>